<commit_message>
Update class for KJC.
</commit_message>
<xml_diff>
--- a/2022/scclac-20220724.xlsx
+++ b/2022/scclac-20220724.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrye/personal/mac/results/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2421463-F9A2-F446-AF5A-94D38EA26A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC9B3A7-B239-E64F-8560-4EEED2F88050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23460" yWindow="500" windowWidth="12340" windowHeight="20480" xr2:uid="{15C3AB5E-E1CD-9F4A-9C99-B5E6C9D2B530}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="65">
   <si>
     <t>class_index</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>Jason Ross</t>
+  </si>
+  <si>
+    <t>ASP</t>
   </si>
 </sst>
 </file>
@@ -586,7 +589,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1091,7 +1094,7 @@
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C45" t="s">
         <v>10</v>

</xml_diff>